<commit_message>
feat: add edp-hrt model
</commit_message>
<xml_diff>
--- a/edp_fix_client/initiator/edp_regression_test/report/edp_report.xlsx
+++ b/edp_fix_client/initiator/edp_regression_test/report/edp_report.xlsx
@@ -570,7 +570,7 @@
       </c>
       <c r="G2" s="5" t="inlineStr">
         <is>
-          <t>9998</t>
+          <t>3002</t>
         </is>
       </c>
       <c r="H2" s="5" t="inlineStr">
@@ -583,10 +583,26 @@
           <t>ERROR_10010062,EDP order rejected due to out of trading hours</t>
         </is>
       </c>
-      <c r="J2" s="5" t="n"/>
-      <c r="K2" s="5" t="n"/>
-      <c r="L2" s="5" t="n"/>
-      <c r="M2" s="5" t="n"/>
+      <c r="J2" s="5" t="inlineStr">
+        <is>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="K2" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L2" s="5" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="M2" s="5" t="inlineStr">
+        <is>
+          <t>ps: 若列表存在failed数据，请查看report.log文件</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="inlineStr">
@@ -621,7 +637,7 @@
       </c>
       <c r="G3" s="5" t="inlineStr">
         <is>
-          <t>1721</t>
+          <t>2980</t>
         </is>
       </c>
       <c r="H3" s="5" t="inlineStr">
@@ -630,9 +646,21 @@
         </is>
       </c>
       <c r="I3" s="5" t="inlineStr"/>
-      <c r="J3" s="5" t="n"/>
-      <c r="K3" s="5" t="n"/>
-      <c r="L3" s="5" t="n"/>
+      <c r="J3" s="5" t="inlineStr">
+        <is>
+          <t>['0', '2', '2']</t>
+        </is>
+      </c>
+      <c r="K3" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L3" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M3" s="5" t="n"/>
     </row>
     <row r="4">
@@ -668,7 +696,7 @@
       </c>
       <c r="G4" s="5" t="inlineStr">
         <is>
-          <t>1721</t>
+          <t>2982</t>
         </is>
       </c>
       <c r="H4" s="5" t="inlineStr">
@@ -677,10 +705,26 @@
         </is>
       </c>
       <c r="I4" s="5" t="inlineStr"/>
-      <c r="J4" s="5" t="n"/>
-      <c r="K4" s="5" t="n"/>
-      <c r="L4" s="5" t="n"/>
-      <c r="M4" s="5" t="n"/>
+      <c r="J4" s="5" t="inlineStr">
+        <is>
+          <t>['0', '2', '2']</t>
+        </is>
+      </c>
+      <c r="K4" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L4" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="M4" s="5" t="inlineStr">
+        <is>
+          <t>FixMsg is OK</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="inlineStr">
@@ -715,7 +759,7 @@
       </c>
       <c r="G5" s="5" t="inlineStr">
         <is>
-          <t>1721</t>
+          <t>2980</t>
         </is>
       </c>
       <c r="H5" s="5" t="inlineStr">
@@ -724,10 +768,26 @@
         </is>
       </c>
       <c r="I5" s="5" t="inlineStr"/>
-      <c r="J5" s="5" t="n"/>
-      <c r="K5" s="5" t="n"/>
-      <c r="L5" s="5" t="n"/>
-      <c r="M5" s="5" t="n"/>
+      <c r="J5" s="5" t="inlineStr">
+        <is>
+          <t>['0', '2', '2']</t>
+        </is>
+      </c>
+      <c r="K5" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L5" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="M5" s="5" t="inlineStr">
+        <is>
+          <t>execType is OK</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="inlineStr">
@@ -762,7 +822,7 @@
       </c>
       <c r="G6" s="5" t="inlineStr">
         <is>
-          <t>1721</t>
+          <t>2982</t>
         </is>
       </c>
       <c r="H6" s="5" t="inlineStr">
@@ -771,9 +831,21 @@
         </is>
       </c>
       <c r="I6" s="5" t="inlineStr"/>
-      <c r="J6" s="5" t="n"/>
-      <c r="K6" s="5" t="n"/>
-      <c r="L6" s="5" t="n"/>
+      <c r="J6" s="5" t="inlineStr">
+        <is>
+          <t>['0', '2', '2']</t>
+        </is>
+      </c>
+      <c r="K6" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L6" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M6" s="5" t="n"/>
     </row>
     <row r="7">
@@ -809,7 +881,7 @@
       </c>
       <c r="G7" s="5" t="inlineStr">
         <is>
-          <t>6028</t>
+          <t>2989</t>
         </is>
       </c>
       <c r="H7" s="5" t="inlineStr">
@@ -818,9 +890,21 @@
         </is>
       </c>
       <c r="I7" s="5" t="inlineStr"/>
-      <c r="J7" s="5" t="n"/>
-      <c r="K7" s="5" t="n"/>
-      <c r="L7" s="5" t="n"/>
+      <c r="J7" s="5" t="inlineStr">
+        <is>
+          <t>['0', '1', '2', '1', '2']</t>
+        </is>
+      </c>
+      <c r="K7" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L7" s="5" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="M7" s="5" t="n"/>
     </row>
     <row r="8">
@@ -856,7 +940,7 @@
       </c>
       <c r="G8" s="5" t="inlineStr">
         <is>
-          <t>6028</t>
+          <t>1308</t>
         </is>
       </c>
       <c r="H8" s="5" t="inlineStr">
@@ -865,9 +949,21 @@
         </is>
       </c>
       <c r="I8" s="5" t="inlineStr"/>
-      <c r="J8" s="5" t="n"/>
-      <c r="K8" s="5" t="n"/>
-      <c r="L8" s="5" t="n"/>
+      <c r="J8" s="5" t="inlineStr">
+        <is>
+          <t>['0', '1', '1', '4']</t>
+        </is>
+      </c>
+      <c r="K8" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L8" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M8" s="5" t="n"/>
     </row>
     <row r="9">
@@ -903,7 +999,7 @@
       </c>
       <c r="G9" s="5" t="inlineStr">
         <is>
-          <t>5110</t>
+          <t>2993</t>
         </is>
       </c>
       <c r="H9" s="5" t="inlineStr">
@@ -912,9 +1008,21 @@
         </is>
       </c>
       <c r="I9" s="5" t="inlineStr"/>
-      <c r="J9" s="5" t="n"/>
-      <c r="K9" s="5" t="n"/>
-      <c r="L9" s="5" t="n"/>
+      <c r="J9" s="5" t="inlineStr">
+        <is>
+          <t>['0', '1', '2', '1', '2']</t>
+        </is>
+      </c>
+      <c r="K9" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L9" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M9" s="5" t="n"/>
     </row>
     <row r="10">
@@ -950,7 +1058,7 @@
       </c>
       <c r="G10" s="5" t="inlineStr">
         <is>
-          <t>5110</t>
+          <t>3154</t>
         </is>
       </c>
       <c r="H10" s="5" t="inlineStr">
@@ -959,9 +1067,21 @@
         </is>
       </c>
       <c r="I10" s="5" t="inlineStr"/>
-      <c r="J10" s="5" t="n"/>
-      <c r="K10" s="5" t="n"/>
-      <c r="L10" s="5" t="n"/>
+      <c r="J10" s="5" t="inlineStr">
+        <is>
+          <t>['0', '1', '2', '2', '1']</t>
+        </is>
+      </c>
+      <c r="K10" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L10" s="5" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="M10" s="5" t="n"/>
     </row>
     <row r="11">
@@ -997,7 +1117,7 @@
       </c>
       <c r="G11" s="5" t="inlineStr">
         <is>
-          <t>1357</t>
+          <t>1499</t>
         </is>
       </c>
       <c r="H11" s="5" t="inlineStr">
@@ -1010,9 +1130,21 @@
           <t>ERROR_30010053,Order rejected due to TOSTNET Cross Reporting failure</t>
         </is>
       </c>
-      <c r="J11" s="5" t="n"/>
-      <c r="K11" s="5" t="n"/>
-      <c r="L11" s="5" t="n"/>
+      <c r="J11" s="5" t="inlineStr">
+        <is>
+          <t>['0', '2', '4', '4']</t>
+        </is>
+      </c>
+      <c r="K11" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L11" s="5" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="M11" s="5" t="n"/>
     </row>
     <row r="12">
@@ -1048,7 +1180,7 @@
       </c>
       <c r="G12" s="5" t="inlineStr">
         <is>
-          <t>1357</t>
+          <t>1321</t>
         </is>
       </c>
       <c r="H12" s="5" t="inlineStr">
@@ -1061,9 +1193,21 @@
           <t>ERROR_30010053,Order rejected due to TOSTNET Cross Reporting failure</t>
         </is>
       </c>
-      <c r="J12" s="5" t="n"/>
-      <c r="K12" s="5" t="n"/>
-      <c r="L12" s="5" t="n"/>
+      <c r="J12" s="5" t="inlineStr">
+        <is>
+          <t>['0', '2', '4', '4']</t>
+        </is>
+      </c>
+      <c r="K12" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L12" s="5" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="M12" s="5" t="n"/>
     </row>
     <row r="13">
@@ -1099,7 +1243,7 @@
       </c>
       <c r="G13" s="5" t="inlineStr">
         <is>
-          <t>1357</t>
+          <t>1499</t>
         </is>
       </c>
       <c r="H13" s="5" t="inlineStr">
@@ -1112,9 +1256,21 @@
           <t>ERROR_30010053,Order rejected due to TOSTNET Cross Reporting failure</t>
         </is>
       </c>
-      <c r="J13" s="5" t="n"/>
-      <c r="K13" s="5" t="n"/>
-      <c r="L13" s="5" t="n"/>
+      <c r="J13" s="5" t="inlineStr">
+        <is>
+          <t>['0', '2', '4', '4']</t>
+        </is>
+      </c>
+      <c r="K13" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L13" s="5" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="M13" s="5" t="n"/>
     </row>
     <row r="14">
@@ -1150,7 +1306,7 @@
       </c>
       <c r="G14" s="5" t="inlineStr">
         <is>
-          <t>1357</t>
+          <t>1321</t>
         </is>
       </c>
       <c r="H14" s="5" t="inlineStr">
@@ -1163,9 +1319,21 @@
           <t>ERROR_30010053,Order rejected due to TOSTNET Cross Reporting failure</t>
         </is>
       </c>
-      <c r="J14" s="5" t="n"/>
-      <c r="K14" s="5" t="n"/>
-      <c r="L14" s="5" t="n"/>
+      <c r="J14" s="5" t="inlineStr">
+        <is>
+          <t>['0', '2', '4', '4']</t>
+        </is>
+      </c>
+      <c r="K14" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L14" s="5" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="M14" s="5" t="n"/>
     </row>
     <row r="15">
@@ -1201,7 +1369,7 @@
       </c>
       <c r="G15" s="5" t="inlineStr">
         <is>
-          <t>1320</t>
+          <t>1496</t>
         </is>
       </c>
       <c r="H15" s="5" t="inlineStr">
@@ -1210,9 +1378,21 @@
         </is>
       </c>
       <c r="I15" s="5" t="inlineStr"/>
-      <c r="J15" s="5" t="n"/>
-      <c r="K15" s="5" t="n"/>
-      <c r="L15" s="5" t="n"/>
+      <c r="J15" s="5" t="inlineStr">
+        <is>
+          <t>['0', '2', '2']</t>
+        </is>
+      </c>
+      <c r="K15" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L15" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M15" s="5" t="n"/>
     </row>
     <row r="16">
@@ -1248,7 +1428,7 @@
       </c>
       <c r="G16" s="5" t="inlineStr">
         <is>
-          <t>1320</t>
+          <t>1496</t>
         </is>
       </c>
       <c r="H16" s="5" t="inlineStr">
@@ -1261,9 +1441,21 @@
           <t>Unknown order</t>
         </is>
       </c>
-      <c r="J16" s="5" t="n"/>
-      <c r="K16" s="5" t="n"/>
-      <c r="L16" s="5" t="n"/>
+      <c r="J16" s="5" t="inlineStr">
+        <is>
+          <t>['8']</t>
+        </is>
+      </c>
+      <c r="K16" s="5" t="inlineStr">
+        <is>
+          <t>Unknown order</t>
+        </is>
+      </c>
+      <c r="L16" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M16" s="5" t="n"/>
     </row>
     <row r="17">
@@ -1299,7 +1491,7 @@
       </c>
       <c r="G17" s="5" t="inlineStr">
         <is>
-          <t>1320</t>
+          <t>2927</t>
         </is>
       </c>
       <c r="H17" s="5" t="inlineStr">
@@ -1308,9 +1500,21 @@
         </is>
       </c>
       <c r="I17" s="5" t="inlineStr"/>
-      <c r="J17" s="5" t="n"/>
-      <c r="K17" s="5" t="n"/>
-      <c r="L17" s="5" t="n"/>
+      <c r="J17" s="5" t="inlineStr">
+        <is>
+          <t>['0', '2', '2']</t>
+        </is>
+      </c>
+      <c r="K17" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L17" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M17" s="5" t="n"/>
     </row>
     <row r="18">
@@ -1346,7 +1550,7 @@
       </c>
       <c r="G18" s="5" t="inlineStr">
         <is>
-          <t>1320</t>
+          <t>2927</t>
         </is>
       </c>
       <c r="H18" s="5" t="inlineStr">
@@ -1359,9 +1563,21 @@
           <t>Unknown order</t>
         </is>
       </c>
-      <c r="J18" s="5" t="n"/>
-      <c r="K18" s="5" t="n"/>
-      <c r="L18" s="5" t="n"/>
+      <c r="J18" s="5" t="inlineStr">
+        <is>
+          <t>['8']</t>
+        </is>
+      </c>
+      <c r="K18" s="5" t="inlineStr">
+        <is>
+          <t>Unknown order</t>
+        </is>
+      </c>
+      <c r="L18" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M18" s="5" t="n"/>
     </row>
     <row r="19">
@@ -1397,7 +1613,7 @@
       </c>
       <c r="G19" s="5" t="inlineStr">
         <is>
-          <t>1321</t>
+          <t>3915</t>
         </is>
       </c>
       <c r="H19" s="5" t="inlineStr">
@@ -1406,9 +1622,21 @@
         </is>
       </c>
       <c r="I19" s="5" t="inlineStr"/>
-      <c r="J19" s="5" t="n"/>
-      <c r="K19" s="5" t="n"/>
-      <c r="L19" s="5" t="n"/>
+      <c r="J19" s="5" t="inlineStr">
+        <is>
+          <t>['0', '1', '1', '4']</t>
+        </is>
+      </c>
+      <c r="K19" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L19" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M19" s="5" t="n"/>
     </row>
     <row r="20">
@@ -1444,7 +1672,7 @@
       </c>
       <c r="G20" s="5" t="inlineStr">
         <is>
-          <t>1321</t>
+          <t>3915</t>
         </is>
       </c>
       <c r="H20" s="5" t="inlineStr">
@@ -1457,9 +1685,21 @@
           <t>Unknown order</t>
         </is>
       </c>
-      <c r="J20" s="5" t="n"/>
-      <c r="K20" s="5" t="n"/>
-      <c r="L20" s="5" t="n"/>
+      <c r="J20" s="5" t="inlineStr">
+        <is>
+          <t>['8']</t>
+        </is>
+      </c>
+      <c r="K20" s="5" t="inlineStr">
+        <is>
+          <t>Unknown order</t>
+        </is>
+      </c>
+      <c r="L20" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M20" s="5" t="n"/>
     </row>
     <row r="21">
@@ -1495,7 +1735,7 @@
       </c>
       <c r="G21" s="5" t="inlineStr">
         <is>
-          <t>1321</t>
+          <t>3916</t>
         </is>
       </c>
       <c r="H21" s="5" t="inlineStr">
@@ -1504,9 +1744,21 @@
         </is>
       </c>
       <c r="I21" s="5" t="inlineStr"/>
-      <c r="J21" s="5" t="n"/>
-      <c r="K21" s="5" t="n"/>
-      <c r="L21" s="5" t="n"/>
+      <c r="J21" s="5" t="inlineStr">
+        <is>
+          <t>['0', '1', '1', '4']</t>
+        </is>
+      </c>
+      <c r="K21" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L21" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M21" s="5" t="n"/>
     </row>
     <row r="22">
@@ -1542,7 +1794,7 @@
       </c>
       <c r="G22" s="5" t="inlineStr">
         <is>
-          <t>1321</t>
+          <t>3916</t>
         </is>
       </c>
       <c r="H22" s="5" t="inlineStr">
@@ -1555,9 +1807,21 @@
           <t>Unknown order</t>
         </is>
       </c>
-      <c r="J22" s="5" t="n"/>
-      <c r="K22" s="5" t="n"/>
-      <c r="L22" s="5" t="n"/>
+      <c r="J22" s="5" t="inlineStr">
+        <is>
+          <t>['8']</t>
+        </is>
+      </c>
+      <c r="K22" s="5" t="inlineStr">
+        <is>
+          <t>Unknown order</t>
+        </is>
+      </c>
+      <c r="L22" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M22" s="5" t="n"/>
     </row>
     <row r="23">
@@ -1593,18 +1857,30 @@
       </c>
       <c r="G23" s="5" t="inlineStr">
         <is>
-          <t>1366</t>
+          <t>1329</t>
         </is>
       </c>
       <c r="H23" s="5" t="inlineStr">
         <is>
-          <t>['0', '2', '4']</t>
+          <t>['0', '2', '4', '4']</t>
         </is>
       </c>
       <c r="I23" s="5" t="inlineStr"/>
-      <c r="J23" s="5" t="n"/>
-      <c r="K23" s="5" t="n"/>
-      <c r="L23" s="5" t="n"/>
+      <c r="J23" s="5" t="inlineStr">
+        <is>
+          <t>['0', '2', '4', '4']</t>
+        </is>
+      </c>
+      <c r="K23" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L23" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M23" s="5" t="n"/>
     </row>
     <row r="24">
@@ -1640,18 +1916,30 @@
       </c>
       <c r="G24" s="5" t="inlineStr">
         <is>
-          <t>1366</t>
+          <t>1346</t>
         </is>
       </c>
       <c r="H24" s="5" t="inlineStr">
         <is>
-          <t>['0', '2', '4']</t>
+          <t>['0', '2', '4', '4']</t>
         </is>
       </c>
       <c r="I24" s="5" t="inlineStr"/>
-      <c r="J24" s="5" t="n"/>
-      <c r="K24" s="5" t="n"/>
-      <c r="L24" s="5" t="n"/>
+      <c r="J24" s="5" t="inlineStr">
+        <is>
+          <t>['0', '2', '4', '4']</t>
+        </is>
+      </c>
+      <c r="K24" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L24" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M24" s="5" t="n"/>
     </row>
     <row r="25">
@@ -1687,18 +1975,30 @@
       </c>
       <c r="G25" s="5" t="inlineStr">
         <is>
-          <t>1366</t>
+          <t>1329</t>
         </is>
       </c>
       <c r="H25" s="5" t="inlineStr">
         <is>
-          <t>['0', '2', '4']</t>
+          <t>['0', '2', '4', '4']</t>
         </is>
       </c>
       <c r="I25" s="5" t="inlineStr"/>
-      <c r="J25" s="5" t="n"/>
-      <c r="K25" s="5" t="n"/>
-      <c r="L25" s="5" t="n"/>
+      <c r="J25" s="5" t="inlineStr">
+        <is>
+          <t>['0', '2', '4', '4']</t>
+        </is>
+      </c>
+      <c r="K25" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L25" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M25" s="5" t="n"/>
     </row>
     <row r="26">
@@ -1734,18 +2034,30 @@
       </c>
       <c r="G26" s="5" t="inlineStr">
         <is>
-          <t>1366</t>
+          <t>1346</t>
         </is>
       </c>
       <c r="H26" s="5" t="inlineStr">
         <is>
-          <t>['0', '2', '4']</t>
+          <t>['0', '2', '4', '4']</t>
         </is>
       </c>
       <c r="I26" s="5" t="inlineStr"/>
-      <c r="J26" s="5" t="n"/>
-      <c r="K26" s="5" t="n"/>
-      <c r="L26" s="5" t="n"/>
+      <c r="J26" s="5" t="inlineStr">
+        <is>
+          <t>['0', '2', '4', '4']</t>
+        </is>
+      </c>
+      <c r="K26" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L26" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M26" s="5" t="n"/>
     </row>
     <row r="27">
@@ -1756,7 +2068,7 @@
       </c>
       <c r="B27" s="5" t="inlineStr">
         <is>
-          <t>Regular Order Flow-G(New Order-&gt; IOCExpired-&gt; Canceled)</t>
+          <t>Regular Order Flow-G(New Order-&gt; ToSTNeT Confirmation-&gt; Canceled)</t>
         </is>
       </c>
       <c r="C27" s="5" t="inlineStr">
@@ -1781,18 +2093,30 @@
       </c>
       <c r="G27" s="5" t="inlineStr">
         <is>
-          <t>1308</t>
+          <t>1496</t>
         </is>
       </c>
       <c r="H27" s="5" t="inlineStr">
         <is>
-          <t>['0', '4']</t>
+          <t>['0', '2', '2']</t>
         </is>
       </c>
       <c r="I27" s="5" t="inlineStr"/>
-      <c r="J27" s="5" t="n"/>
-      <c r="K27" s="5" t="n"/>
-      <c r="L27" s="5" t="n"/>
+      <c r="J27" s="5" t="inlineStr">
+        <is>
+          <t>['0', '2', '2']</t>
+        </is>
+      </c>
+      <c r="K27" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L27" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M27" s="5" t="n"/>
     </row>
     <row r="28">
@@ -1828,7 +2152,7 @@
       </c>
       <c r="G28" s="5" t="inlineStr">
         <is>
-          <t>1308</t>
+          <t>1496</t>
         </is>
       </c>
       <c r="H28" s="5" t="inlineStr">
@@ -1841,9 +2165,21 @@
           <t>Unknown order</t>
         </is>
       </c>
-      <c r="J28" s="5" t="n"/>
-      <c r="K28" s="5" t="n"/>
-      <c r="L28" s="5" t="n"/>
+      <c r="J28" s="5" t="inlineStr">
+        <is>
+          <t>['8']</t>
+        </is>
+      </c>
+      <c r="K28" s="5" t="inlineStr">
+        <is>
+          <t>Unknown order</t>
+        </is>
+      </c>
+      <c r="L28" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M28" s="5" t="n"/>
     </row>
     <row r="29">
@@ -1879,18 +2215,30 @@
       </c>
       <c r="G29" s="5" t="inlineStr">
         <is>
-          <t>1308</t>
+          <t>2927</t>
         </is>
       </c>
       <c r="H29" s="5" t="inlineStr">
         <is>
-          <t>['0', '4']</t>
+          <t>['0', '2', '2']</t>
         </is>
       </c>
       <c r="I29" s="5" t="inlineStr"/>
-      <c r="J29" s="5" t="n"/>
-      <c r="K29" s="5" t="n"/>
-      <c r="L29" s="5" t="n"/>
+      <c r="J29" s="5" t="inlineStr">
+        <is>
+          <t>['0', '2', '2']</t>
+        </is>
+      </c>
+      <c r="K29" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L29" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M29" s="5" t="n"/>
     </row>
     <row r="30">
@@ -1926,7 +2274,7 @@
       </c>
       <c r="G30" s="5" t="inlineStr">
         <is>
-          <t>1308</t>
+          <t>2927</t>
         </is>
       </c>
       <c r="H30" s="5" t="inlineStr">
@@ -1939,9 +2287,21 @@
           <t>Unknown order</t>
         </is>
       </c>
-      <c r="J30" s="5" t="n"/>
-      <c r="K30" s="5" t="n"/>
-      <c r="L30" s="5" t="n"/>
+      <c r="J30" s="5" t="inlineStr">
+        <is>
+          <t>['8']</t>
+        </is>
+      </c>
+      <c r="K30" s="5" t="inlineStr">
+        <is>
+          <t>Unknown order</t>
+        </is>
+      </c>
+      <c r="L30" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M30" s="5" t="n"/>
     </row>
     <row r="31">
@@ -1977,18 +2337,30 @@
       </c>
       <c r="G31" s="5" t="inlineStr">
         <is>
-          <t>1308</t>
+          <t>3915</t>
         </is>
       </c>
       <c r="H31" s="5" t="inlineStr">
         <is>
-          <t>['0', '4']</t>
+          <t>['0', '2', '2']</t>
         </is>
       </c>
       <c r="I31" s="5" t="inlineStr"/>
-      <c r="J31" s="5" t="n"/>
-      <c r="K31" s="5" t="n"/>
-      <c r="L31" s="5" t="n"/>
+      <c r="J31" s="5" t="inlineStr">
+        <is>
+          <t>['0', '2', '2']</t>
+        </is>
+      </c>
+      <c r="K31" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L31" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M31" s="5" t="n"/>
     </row>
     <row r="32">
@@ -2024,7 +2396,7 @@
       </c>
       <c r="G32" s="5" t="inlineStr">
         <is>
-          <t>1308</t>
+          <t>3915</t>
         </is>
       </c>
       <c r="H32" s="5" t="inlineStr">
@@ -2037,9 +2409,21 @@
           <t>Unknown order</t>
         </is>
       </c>
-      <c r="J32" s="5" t="n"/>
-      <c r="K32" s="5" t="n"/>
-      <c r="L32" s="5" t="n"/>
+      <c r="J32" s="5" t="inlineStr">
+        <is>
+          <t>['8']</t>
+        </is>
+      </c>
+      <c r="K32" s="5" t="inlineStr">
+        <is>
+          <t>Unknown order</t>
+        </is>
+      </c>
+      <c r="L32" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M32" s="5" t="n"/>
     </row>
     <row r="33">
@@ -2075,18 +2459,30 @@
       </c>
       <c r="G33" s="5" t="inlineStr">
         <is>
-          <t>1308</t>
+          <t>3916</t>
         </is>
       </c>
       <c r="H33" s="5" t="inlineStr">
         <is>
-          <t>['0', '4']</t>
+          <t>['0', '2', '2']</t>
         </is>
       </c>
       <c r="I33" s="5" t="inlineStr"/>
-      <c r="J33" s="5" t="n"/>
-      <c r="K33" s="5" t="n"/>
-      <c r="L33" s="5" t="n"/>
+      <c r="J33" s="5" t="inlineStr">
+        <is>
+          <t>['0', '1', '1', '1', '1', '4']</t>
+        </is>
+      </c>
+      <c r="K33" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L33" s="5" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="M33" s="5" t="n"/>
     </row>
     <row r="34">
@@ -2122,7 +2518,7 @@
       </c>
       <c r="G34" s="5" t="inlineStr">
         <is>
-          <t>1308</t>
+          <t>3916</t>
         </is>
       </c>
       <c r="H34" s="5" t="inlineStr">
@@ -2135,9 +2531,21 @@
           <t>Unknown order</t>
         </is>
       </c>
-      <c r="J34" s="5" t="n"/>
-      <c r="K34" s="5" t="n"/>
-      <c r="L34" s="5" t="n"/>
+      <c r="J34" s="5" t="inlineStr">
+        <is>
+          <t>['8']</t>
+        </is>
+      </c>
+      <c r="K34" s="5" t="inlineStr">
+        <is>
+          <t>Unknown order</t>
+        </is>
+      </c>
+      <c r="L34" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M34" s="5" t="n"/>
     </row>
     <row r="35">
@@ -2182,9 +2590,21 @@
         </is>
       </c>
       <c r="I35" s="5" t="inlineStr"/>
-      <c r="J35" s="5" t="n"/>
-      <c r="K35" s="5" t="n"/>
-      <c r="L35" s="5" t="n"/>
+      <c r="J35" s="5" t="inlineStr">
+        <is>
+          <t>['8']</t>
+        </is>
+      </c>
+      <c r="K35" s="5" t="inlineStr">
+        <is>
+          <t>ERROR_20010063,Order rejected due to SOR Limit Price Control, sor_price=701.5 exceeds TSE_High=701</t>
+        </is>
+      </c>
+      <c r="L35" s="5" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="M35" s="5" t="n"/>
     </row>
     <row r="36">
@@ -2229,9 +2649,21 @@
         </is>
       </c>
       <c r="I36" s="5" t="inlineStr"/>
-      <c r="J36" s="5" t="n"/>
-      <c r="K36" s="5" t="n"/>
-      <c r="L36" s="5" t="n"/>
+      <c r="J36" s="5" t="inlineStr">
+        <is>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="K36" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L36" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M36" s="5" t="n"/>
     </row>
     <row r="37">
@@ -2276,9 +2708,21 @@
         </is>
       </c>
       <c r="I37" s="5" t="inlineStr"/>
-      <c r="J37" s="5" t="n"/>
-      <c r="K37" s="5" t="n"/>
-      <c r="L37" s="5" t="n"/>
+      <c r="J37" s="5" t="inlineStr">
+        <is>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="K37" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L37" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M37" s="5" t="n"/>
     </row>
     <row r="38">
@@ -2323,9 +2767,21 @@
         </is>
       </c>
       <c r="I38" s="5" t="inlineStr"/>
-      <c r="J38" s="5" t="n"/>
-      <c r="K38" s="5" t="n"/>
-      <c r="L38" s="5" t="n"/>
+      <c r="J38" s="5" t="inlineStr">
+        <is>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="K38" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L38" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M38" s="5" t="n"/>
     </row>
     <row r="39">
@@ -2374,9 +2830,21 @@
           <t>ERROR_10010013,No available instrument risk check data found</t>
         </is>
       </c>
-      <c r="J39" s="5" t="n"/>
-      <c r="K39" s="5" t="n"/>
-      <c r="L39" s="5" t="n"/>
+      <c r="J39" s="5" t="inlineStr">
+        <is>
+          <t>['8']</t>
+        </is>
+      </c>
+      <c r="K39" s="5" t="inlineStr">
+        <is>
+          <t>ERROR_10010013,No available instrument risk check data found: instrumentDate=not_found,expectedDate=20231020</t>
+        </is>
+      </c>
+      <c r="L39" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M39" s="5" t="n"/>
     </row>
     <row r="40">
@@ -2412,7 +2880,7 @@
       </c>
       <c r="G40" s="5" t="inlineStr">
         <is>
-          <t>1324</t>
+          <t>2980</t>
         </is>
       </c>
       <c r="H40" s="5" t="inlineStr">
@@ -2425,9 +2893,21 @@
           <t>ERROR_10010014,Price exceeds the high - low price range</t>
         </is>
       </c>
-      <c r="J40" s="5" t="n"/>
-      <c r="K40" s="5" t="n"/>
-      <c r="L40" s="5" t="n"/>
+      <c r="J40" s="5" t="inlineStr">
+        <is>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="K40" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L40" s="5" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="M40" s="5" t="n"/>
     </row>
     <row r="41">
@@ -2463,7 +2943,7 @@
       </c>
       <c r="G41" s="5" t="inlineStr">
         <is>
-          <t>1324</t>
+          <t>2980</t>
         </is>
       </c>
       <c r="H41" s="5" t="inlineStr">
@@ -2476,9 +2956,21 @@
           <t>ERROR_10010014,Price exceeds the high - low price range</t>
         </is>
       </c>
-      <c r="J41" s="5" t="n"/>
-      <c r="K41" s="5" t="n"/>
-      <c r="L41" s="5" t="n"/>
+      <c r="J41" s="5" t="inlineStr">
+        <is>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="K41" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L41" s="5" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="M41" s="5" t="n"/>
     </row>
     <row r="42">
@@ -2519,17 +3011,25 @@
       </c>
       <c r="H42" s="5" t="inlineStr">
         <is>
-          <t>['8']</t>
-        </is>
-      </c>
-      <c r="I42" s="5" t="inlineStr">
-        <is>
-          <t>ERROR_10010015,Tick-size is not matched with small tick</t>
-        </is>
-      </c>
-      <c r="J42" s="5" t="n"/>
-      <c r="K42" s="5" t="n"/>
-      <c r="L42" s="5" t="n"/>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="I42" s="5" t="inlineStr"/>
+      <c r="J42" s="5" t="inlineStr">
+        <is>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="K42" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L42" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M42" s="5" t="n"/>
     </row>
     <row r="43">
@@ -2570,17 +3070,25 @@
       </c>
       <c r="H43" s="5" t="inlineStr">
         <is>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="I43" s="5" t="inlineStr"/>
+      <c r="J43" s="5" t="inlineStr">
+        <is>
           <t>['8']</t>
         </is>
       </c>
-      <c r="I43" s="5" t="inlineStr">
-        <is>
-          <t>ERROR_10010015,Tick-size is not matched with small tick</t>
-        </is>
-      </c>
-      <c r="J43" s="5" t="n"/>
-      <c r="K43" s="5" t="n"/>
-      <c r="L43" s="5" t="n"/>
+      <c r="K43" s="5" t="inlineStr">
+        <is>
+          <t>ERROR_20010063,Order rejected due to SOR Limit Price Control, sor_price=1825 exceeds TSE_Low=1825.5</t>
+        </is>
+      </c>
+      <c r="L43" s="5" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="M43" s="5" t="n"/>
     </row>
     <row r="44">
@@ -2621,17 +3129,25 @@
       </c>
       <c r="H44" s="5" t="inlineStr">
         <is>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="I44" s="5" t="inlineStr"/>
+      <c r="J44" s="5" t="inlineStr">
+        <is>
           <t>['8']</t>
         </is>
       </c>
-      <c r="I44" s="5" t="inlineStr">
-        <is>
-          <t>ERROR_10010015,Tick-size is not matched with small tick</t>
-        </is>
-      </c>
-      <c r="J44" s="5" t="n"/>
-      <c r="K44" s="5" t="n"/>
-      <c r="L44" s="5" t="n"/>
+      <c r="K44" s="5" t="inlineStr">
+        <is>
+          <t>ERROR_20010037,Order rejected due to special quote: symbol=6965</t>
+        </is>
+      </c>
+      <c r="L44" s="5" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="M44" s="5" t="n"/>
     </row>
     <row r="45">
@@ -2672,17 +3188,25 @@
       </c>
       <c r="H45" s="5" t="inlineStr">
         <is>
-          <t>['8']</t>
-        </is>
-      </c>
-      <c r="I45" s="5" t="inlineStr">
-        <is>
-          <t>ERROR_10010015,Tick-size is not matched with small tick</t>
-        </is>
-      </c>
-      <c r="J45" s="5" t="n"/>
-      <c r="K45" s="5" t="n"/>
-      <c r="L45" s="5" t="n"/>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="I45" s="5" t="inlineStr"/>
+      <c r="J45" s="5" t="inlineStr">
+        <is>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="K45" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L45" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M45" s="5" t="n"/>
     </row>
     <row r="46">
@@ -2723,17 +3247,25 @@
       </c>
       <c r="H46" s="5" t="inlineStr">
         <is>
-          <t>['8']</t>
-        </is>
-      </c>
-      <c r="I46" s="5" t="inlineStr">
-        <is>
-          <t>ERROR_10010015,Tick-size is not matched with small tick</t>
-        </is>
-      </c>
-      <c r="J46" s="5" t="n"/>
-      <c r="K46" s="5" t="n"/>
-      <c r="L46" s="5" t="n"/>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="I46" s="5" t="inlineStr"/>
+      <c r="J46" s="5" t="inlineStr">
+        <is>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="K46" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L46" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M46" s="5" t="n"/>
     </row>
     <row r="47">
@@ -2774,17 +3306,25 @@
       </c>
       <c r="H47" s="5" t="inlineStr">
         <is>
-          <t>['8']</t>
-        </is>
-      </c>
-      <c r="I47" s="5" t="inlineStr">
-        <is>
-          <t>ERROR_10010016,Tick-size is not matched with non-small tick</t>
-        </is>
-      </c>
-      <c r="J47" s="5" t="n"/>
-      <c r="K47" s="5" t="n"/>
-      <c r="L47" s="5" t="n"/>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="I47" s="5" t="inlineStr"/>
+      <c r="J47" s="5" t="inlineStr">
+        <is>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="K47" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L47" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M47" s="5" t="n"/>
     </row>
     <row r="48">
@@ -2825,17 +3365,25 @@
       </c>
       <c r="H48" s="5" t="inlineStr">
         <is>
-          <t>['8']</t>
-        </is>
-      </c>
-      <c r="I48" s="5" t="inlineStr">
-        <is>
-          <t>ERROR_10010016,Tick-size is not matched with non-small tick</t>
-        </is>
-      </c>
-      <c r="J48" s="5" t="n"/>
-      <c r="K48" s="5" t="n"/>
-      <c r="L48" s="5" t="n"/>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="I48" s="5" t="inlineStr"/>
+      <c r="J48" s="5" t="inlineStr">
+        <is>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="K48" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L48" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M48" s="5" t="n"/>
     </row>
     <row r="49">
@@ -2876,7 +3424,7 @@
       </c>
       <c r="H49" s="5" t="inlineStr">
         <is>
-          <t>['8']</t>
+          <t>['0', '4']</t>
         </is>
       </c>
       <c r="I49" s="5" t="inlineStr">
@@ -2884,9 +3432,21 @@
           <t>ERROR_10010016,Tick-size is not matched with non-small tick</t>
         </is>
       </c>
-      <c r="J49" s="5" t="n"/>
-      <c r="K49" s="5" t="n"/>
-      <c r="L49" s="5" t="n"/>
+      <c r="J49" s="5" t="inlineStr">
+        <is>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="K49" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L49" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M49" s="5" t="n"/>
     </row>
     <row r="50">
@@ -2927,7 +3487,7 @@
       </c>
       <c r="H50" s="5" t="inlineStr">
         <is>
-          <t>['8']</t>
+          <t>['0', '4']</t>
         </is>
       </c>
       <c r="I50" s="5" t="inlineStr">
@@ -2935,9 +3495,21 @@
           <t>ERROR_10010016,Tick-size is not matched with non-small tick</t>
         </is>
       </c>
-      <c r="J50" s="5" t="n"/>
-      <c r="K50" s="5" t="n"/>
-      <c r="L50" s="5" t="n"/>
+      <c r="J50" s="5" t="inlineStr">
+        <is>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="K50" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L50" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M50" s="5" t="n"/>
     </row>
     <row r="51">
@@ -2978,7 +3550,7 @@
       </c>
       <c r="H51" s="5" t="inlineStr">
         <is>
-          <t>['8']</t>
+          <t>['0', '4']</t>
         </is>
       </c>
       <c r="I51" s="5" t="inlineStr">
@@ -2986,9 +3558,21 @@
           <t>ERROR_10010016,Tick-size is not matched with non-small tick</t>
         </is>
       </c>
-      <c r="J51" s="5" t="n"/>
-      <c r="K51" s="5" t="n"/>
-      <c r="L51" s="5" t="n"/>
+      <c r="J51" s="5" t="inlineStr">
+        <is>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="K51" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L51" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M51" s="5" t="n"/>
     </row>
     <row r="52">
@@ -3029,7 +3613,7 @@
       </c>
       <c r="H52" s="5" t="inlineStr">
         <is>
-          <t>['8']</t>
+          <t>['0', '4']</t>
         </is>
       </c>
       <c r="I52" s="5" t="inlineStr">
@@ -3037,9 +3621,21 @@
           <t>ERROR_10010016,Tick-size is not matched with non-small tick</t>
         </is>
       </c>
-      <c r="J52" s="5" t="n"/>
-      <c r="K52" s="5" t="n"/>
-      <c r="L52" s="5" t="n"/>
+      <c r="J52" s="5" t="inlineStr">
+        <is>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="K52" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L52" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M52" s="5" t="n"/>
     </row>
     <row r="53">
@@ -3088,9 +3684,21 @@
           <t>ERROR_10010018,Invalid quantity or lot_size</t>
         </is>
       </c>
-      <c r="J53" s="5" t="n"/>
-      <c r="K53" s="5" t="n"/>
-      <c r="L53" s="5" t="n"/>
+      <c r="J53" s="5" t="inlineStr">
+        <is>
+          <t>['8']</t>
+        </is>
+      </c>
+      <c r="K53" s="5" t="inlineStr">
+        <is>
+          <t>ERROR_10010018,Invalid quantity or lot_size: quantity=99,lot_size=100</t>
+        </is>
+      </c>
+      <c r="L53" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M53" s="5" t="n"/>
     </row>
     <row r="54">
@@ -3139,9 +3747,21 @@
           <t>ERROR_10010018,Invalid quantity or lot_size</t>
         </is>
       </c>
-      <c r="J54" s="5" t="n"/>
-      <c r="K54" s="5" t="n"/>
-      <c r="L54" s="5" t="n"/>
+      <c r="J54" s="5" t="inlineStr">
+        <is>
+          <t>['8']</t>
+        </is>
+      </c>
+      <c r="K54" s="5" t="inlineStr">
+        <is>
+          <t>ERROR_10010018,Invalid quantity or lot_size: quantity=0,lot_size=100</t>
+        </is>
+      </c>
+      <c r="L54" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M54" s="5" t="n"/>
     </row>
     <row r="55">
@@ -3186,9 +3806,21 @@
         </is>
       </c>
       <c r="I55" s="5" t="inlineStr"/>
-      <c r="J55" s="5" t="n"/>
-      <c r="K55" s="5" t="n"/>
-      <c r="L55" s="5" t="n"/>
+      <c r="J55" s="5" t="inlineStr">
+        <is>
+          <t>['0', '2', '2']</t>
+        </is>
+      </c>
+      <c r="K55" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L55" s="5" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="M55" s="5" t="n"/>
     </row>
     <row r="56">
@@ -3233,9 +3865,21 @@
         </is>
       </c>
       <c r="I56" s="5" t="inlineStr"/>
-      <c r="J56" s="5" t="n"/>
-      <c r="K56" s="5" t="n"/>
-      <c r="L56" s="5" t="n"/>
+      <c r="J56" s="5" t="inlineStr">
+        <is>
+          <t>['0', '2', '2']</t>
+        </is>
+      </c>
+      <c r="K56" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L56" s="5" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="M56" s="5" t="n"/>
     </row>
     <row r="57">
@@ -3284,9 +3928,21 @@
           <t>ERROR_10010018,Invalid quantity or lot_size</t>
         </is>
       </c>
-      <c r="J57" s="5" t="n"/>
-      <c r="K57" s="5" t="n"/>
-      <c r="L57" s="5" t="n"/>
+      <c r="J57" s="5" t="inlineStr">
+        <is>
+          <t>['8']</t>
+        </is>
+      </c>
+      <c r="K57" s="5" t="inlineStr">
+        <is>
+          <t>ERROR_10010018,Invalid quantity or lot_size: quantity=101,lot_size=100</t>
+        </is>
+      </c>
+      <c r="L57" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M57" s="5" t="n"/>
     </row>
     <row r="58">
@@ -3331,9 +3987,21 @@
         </is>
       </c>
       <c r="I58" s="5" t="inlineStr"/>
-      <c r="J58" s="5" t="n"/>
-      <c r="K58" s="5" t="n"/>
-      <c r="L58" s="5" t="n"/>
+      <c r="J58" s="5" t="inlineStr">
+        <is>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="K58" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L58" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M58" s="5" t="n"/>
     </row>
     <row r="59">
@@ -3378,9 +4046,21 @@
         </is>
       </c>
       <c r="I59" s="5" t="inlineStr"/>
-      <c r="J59" s="5" t="n"/>
-      <c r="K59" s="5" t="n"/>
-      <c r="L59" s="5" t="n"/>
+      <c r="J59" s="5" t="inlineStr">
+        <is>
+          <t>['8']</t>
+        </is>
+      </c>
+      <c r="K59" s="5" t="inlineStr">
+        <is>
+          <t>ERROR_20010063,Order rejected due to SOR Limit Price Control, sor_price=17000 exceeds TSE_Low=17090</t>
+        </is>
+      </c>
+      <c r="L59" s="5" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="M59" s="5" t="n"/>
     </row>
     <row r="60">
@@ -3425,9 +4105,21 @@
         </is>
       </c>
       <c r="I60" s="5" t="inlineStr"/>
-      <c r="J60" s="5" t="n"/>
-      <c r="K60" s="5" t="n"/>
-      <c r="L60" s="5" t="n"/>
+      <c r="J60" s="5" t="inlineStr">
+        <is>
+          <t>['8']</t>
+        </is>
+      </c>
+      <c r="K60" s="5" t="inlineStr">
+        <is>
+          <t>ERROR_20010024,Failed to get TSE High to set price for market order</t>
+        </is>
+      </c>
+      <c r="L60" s="5" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="M60" s="5" t="n"/>
     </row>
     <row r="61">
@@ -3472,9 +4164,21 @@
         </is>
       </c>
       <c r="I61" s="5" t="inlineStr"/>
-      <c r="J61" s="5" t="n"/>
-      <c r="K61" s="5" t="n"/>
-      <c r="L61" s="5" t="n"/>
+      <c r="J61" s="5" t="inlineStr">
+        <is>
+          <t>['8']</t>
+        </is>
+      </c>
+      <c r="K61" s="5" t="inlineStr">
+        <is>
+          <t>ERROR_20010024,Failed to get TSE High to set price for market order</t>
+        </is>
+      </c>
+      <c r="L61" s="5" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="M61" s="5" t="n"/>
     </row>
     <row r="62">
@@ -3523,9 +4227,21 @@
           <t>ERROR_10010018,Invalid quantity or lot_size</t>
         </is>
       </c>
-      <c r="J62" s="5" t="n"/>
-      <c r="K62" s="5" t="n"/>
-      <c r="L62" s="5" t="n"/>
+      <c r="J62" s="5" t="inlineStr">
+        <is>
+          <t>['8']</t>
+        </is>
+      </c>
+      <c r="K62" s="5" t="inlineStr">
+        <is>
+          <t>ERROR_10010018,Invalid quantity or lot_size: quantity=1001,lot_size=1000</t>
+        </is>
+      </c>
+      <c r="L62" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M62" s="5" t="n"/>
     </row>
     <row r="63">
@@ -3574,9 +4290,21 @@
           <t>ERROR_10010011,Notional limit is exceeded</t>
         </is>
       </c>
-      <c r="J63" s="5" t="n"/>
-      <c r="K63" s="5" t="n"/>
-      <c r="L63" s="5" t="n"/>
+      <c r="J63" s="5" t="inlineStr">
+        <is>
+          <t>['8']</t>
+        </is>
+      </c>
+      <c r="K63" s="5" t="inlineStr">
+        <is>
+          <t>ERROR_20010024,Failed to get TSE High to set price for market order</t>
+        </is>
+      </c>
+      <c r="L63" s="5" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="M63" s="5" t="n"/>
     </row>
     <row r="64">
@@ -3625,9 +4353,21 @@
           <t>ERROR_10010003,OrdType is not supported</t>
         </is>
       </c>
-      <c r="J64" s="5" t="n"/>
-      <c r="K64" s="5" t="n"/>
-      <c r="L64" s="5" t="n"/>
+      <c r="J64" s="5" t="inlineStr">
+        <is>
+          <t>['8']</t>
+        </is>
+      </c>
+      <c r="K64" s="5" t="inlineStr">
+        <is>
+          <t>ERROR_10010003,OrdType is not supported: ordType=9</t>
+        </is>
+      </c>
+      <c r="L64" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M64" s="5" t="n"/>
     </row>
     <row r="65">
@@ -3676,9 +4416,21 @@
           <t>ERROR_10010012,TimeInForce is not supported</t>
         </is>
       </c>
-      <c r="J65" s="5" t="n"/>
-      <c r="K65" s="5" t="n"/>
-      <c r="L65" s="5" t="n"/>
+      <c r="J65" s="5" t="inlineStr">
+        <is>
+          <t>['8']</t>
+        </is>
+      </c>
+      <c r="K65" s="5" t="inlineStr">
+        <is>
+          <t>ERROR_10010012,TimeInForce is not supported: timeInForce=6</t>
+        </is>
+      </c>
+      <c r="L65" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M65" s="5" t="n"/>
     </row>
     <row r="66">
@@ -3727,9 +4479,21 @@
           <t>ERROR_10010004,Side is not supported</t>
         </is>
       </c>
-      <c r="J66" s="5" t="n"/>
-      <c r="K66" s="5" t="n"/>
-      <c r="L66" s="5" t="n"/>
+      <c r="J66" s="5" t="inlineStr">
+        <is>
+          <t>['8']</t>
+        </is>
+      </c>
+      <c r="K66" s="5" t="inlineStr">
+        <is>
+          <t>ERROR_10010004,Side is not supported: side=5</t>
+        </is>
+      </c>
+      <c r="L66" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M66" s="5" t="n"/>
     </row>
     <row r="67">
@@ -3778,9 +4542,21 @@
           <t>ERROR_10010009,Invalid account</t>
         </is>
       </c>
-      <c r="J67" s="5" t="n"/>
-      <c r="K67" s="5" t="n"/>
-      <c r="L67" s="5" t="n"/>
+      <c r="J67" s="5" t="inlineStr">
+        <is>
+          <t>['8']</t>
+        </is>
+      </c>
+      <c r="K67" s="5" t="inlineStr">
+        <is>
+          <t>ERROR_10010009,Invalid account: senderCompID=RUAT_EDP_5, account=RUAT_EDP_ACCOUNT_53</t>
+        </is>
+      </c>
+      <c r="L67" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M67" s="5" t="n"/>
     </row>
     <row r="68">
@@ -3829,9 +4605,21 @@
           <t>ERROR_10010025,Rule80A is not supported</t>
         </is>
       </c>
-      <c r="J68" s="5" t="n"/>
-      <c r="K68" s="5" t="n"/>
-      <c r="L68" s="5" t="n"/>
+      <c r="J68" s="5" t="inlineStr">
+        <is>
+          <t>['8']</t>
+        </is>
+      </c>
+      <c r="K68" s="5" t="inlineStr">
+        <is>
+          <t>ERROR_10010025,Rule80A is not supported: rule80A=S</t>
+        </is>
+      </c>
+      <c r="L68" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M68" s="5" t="n"/>
     </row>
     <row r="69">
@@ -3880,9 +4668,21 @@
           <t>ERROR_10010026,CashMargin is not supported</t>
         </is>
       </c>
-      <c r="J69" s="5" t="n"/>
-      <c r="K69" s="5" t="n"/>
-      <c r="L69" s="5" t="n"/>
+      <c r="J69" s="5" t="inlineStr">
+        <is>
+          <t>['8']</t>
+        </is>
+      </c>
+      <c r="K69" s="5" t="inlineStr">
+        <is>
+          <t>ERROR_10010026,CashMargin is not supported: cashMargin=2</t>
+        </is>
+      </c>
+      <c r="L69" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M69" s="5" t="n"/>
     </row>
     <row r="70">
@@ -3931,9 +4731,21 @@
           <t>ERROR_10010027,MarginTransactionType is not supported</t>
         </is>
       </c>
-      <c r="J70" s="5" t="n"/>
-      <c r="K70" s="5" t="n"/>
-      <c r="L70" s="5" t="n"/>
+      <c r="J70" s="5" t="inlineStr">
+        <is>
+          <t>['8']</t>
+        </is>
+      </c>
+      <c r="K70" s="5" t="inlineStr">
+        <is>
+          <t>ERROR_10010027,MarginTransactionType is not supported: marginTransactionType=1</t>
+        </is>
+      </c>
+      <c r="L70" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M70" s="5" t="n"/>
     </row>
     <row r="71">
@@ -3982,9 +4794,21 @@
           <t>ERROR_10010028,CrossingPriceType is not supported</t>
         </is>
       </c>
-      <c r="J71" s="5" t="n"/>
-      <c r="K71" s="5" t="n"/>
-      <c r="L71" s="5" t="n"/>
+      <c r="J71" s="5" t="inlineStr">
+        <is>
+          <t>['8']</t>
+        </is>
+      </c>
+      <c r="K71" s="5" t="inlineStr">
+        <is>
+          <t>ERROR_10010028,CrossingPriceType is not supported: crossingPriceType=ROL</t>
+        </is>
+      </c>
+      <c r="L71" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M71" s="5" t="n"/>
     </row>
     <row r="72">
@@ -4029,9 +4853,21 @@
         </is>
       </c>
       <c r="I72" s="5" t="inlineStr"/>
-      <c r="J72" s="5" t="n"/>
-      <c r="K72" s="5" t="n"/>
-      <c r="L72" s="5" t="n"/>
+      <c r="J72" s="5" t="inlineStr">
+        <is>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="K72" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L72" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M72" s="5" t="n"/>
     </row>
     <row r="73">
@@ -4076,9 +4912,21 @@
         </is>
       </c>
       <c r="I73" s="5" t="inlineStr"/>
-      <c r="J73" s="5" t="n"/>
-      <c r="K73" s="5" t="n"/>
-      <c r="L73" s="5" t="n"/>
+      <c r="J73" s="5" t="inlineStr">
+        <is>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="K73" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L73" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M73" s="5" t="n"/>
     </row>
     <row r="74">
@@ -4123,9 +4971,21 @@
         </is>
       </c>
       <c r="I74" s="5" t="inlineStr"/>
-      <c r="J74" s="5" t="n"/>
-      <c r="K74" s="5" t="n"/>
-      <c r="L74" s="5" t="n"/>
+      <c r="J74" s="5" t="inlineStr">
+        <is>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="K74" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L74" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M74" s="5" t="n"/>
     </row>
     <row r="75">
@@ -4170,9 +5030,21 @@
         </is>
       </c>
       <c r="I75" s="5" t="inlineStr"/>
-      <c r="J75" s="5" t="n"/>
-      <c r="K75" s="5" t="n"/>
-      <c r="L75" s="5" t="n"/>
+      <c r="J75" s="5" t="inlineStr">
+        <is>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="K75" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L75" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M75" s="5" t="n"/>
     </row>
     <row r="76">
@@ -4217,9 +5089,21 @@
         </is>
       </c>
       <c r="I76" s="5" t="inlineStr"/>
-      <c r="J76" s="5" t="n"/>
-      <c r="K76" s="5" t="n"/>
-      <c r="L76" s="5" t="n"/>
+      <c r="J76" s="5" t="inlineStr">
+        <is>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="K76" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L76" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M76" s="5" t="n"/>
     </row>
     <row r="77">
@@ -4264,9 +5148,21 @@
         </is>
       </c>
       <c r="I77" s="5" t="inlineStr"/>
-      <c r="J77" s="5" t="n"/>
-      <c r="K77" s="5" t="n"/>
-      <c r="L77" s="5" t="n"/>
+      <c r="J77" s="5" t="inlineStr">
+        <is>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="K77" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L77" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M77" s="5" t="n"/>
     </row>
     <row r="78">
@@ -4311,9 +5207,21 @@
         </is>
       </c>
       <c r="I78" s="5" t="inlineStr"/>
-      <c r="J78" s="5" t="n"/>
-      <c r="K78" s="5" t="n"/>
-      <c r="L78" s="5" t="n"/>
+      <c r="J78" s="5" t="inlineStr">
+        <is>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="K78" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L78" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M78" s="5" t="n"/>
     </row>
     <row r="79">
@@ -4358,9 +5266,21 @@
         </is>
       </c>
       <c r="I79" s="5" t="inlineStr"/>
-      <c r="J79" s="5" t="n"/>
-      <c r="K79" s="5" t="n"/>
-      <c r="L79" s="5" t="n"/>
+      <c r="J79" s="5" t="inlineStr">
+        <is>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="K79" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L79" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M79" s="5" t="n"/>
     </row>
     <row r="80">
@@ -4405,9 +5325,21 @@
         </is>
       </c>
       <c r="I80" s="5" t="inlineStr"/>
-      <c r="J80" s="5" t="n"/>
-      <c r="K80" s="5" t="n"/>
-      <c r="L80" s="5" t="n"/>
+      <c r="J80" s="5" t="inlineStr">
+        <is>
+          <t>['0', '4']</t>
+        </is>
+      </c>
+      <c r="K80" s="5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L80" s="5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
       <c r="M80" s="5" t="n"/>
     </row>
   </sheetData>

</xml_diff>